<commit_message>
Product Backlog updated, Scrum backlogs defined.
</commit_message>
<xml_diff>
--- a/SEM Coursework Backlog.xlsx
+++ b/SEM Coursework Backlog.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\napier-mail.napier.ac.uk\students\school of computing\user data\40314579\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hubert\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{085856FC-AFF1-414C-A71F-585B8EF2AFAC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9600"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="39">
   <si>
     <t>ID</t>
   </si>
@@ -44,9 +45,6 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>Product Backlog</t>
-  </si>
-  <si>
     <t>Git Hub</t>
   </si>
   <si>
@@ -59,9 +57,6 @@
     <t>2 weeks</t>
   </si>
   <si>
-    <t>Updates through Entireity of Project</t>
-  </si>
-  <si>
     <t>Ten mintues</t>
   </si>
   <si>
@@ -81,12 +76,78 @@
   </si>
   <si>
     <t>Three Weeks</t>
+  </si>
+  <si>
+    <t>Sprint</t>
+  </si>
+  <si>
+    <t>1st Sprint - weeks 1-3</t>
+  </si>
+  <si>
+    <t>1st</t>
+  </si>
+  <si>
+    <t>2nd</t>
+  </si>
+  <si>
+    <t>3rd</t>
+  </si>
+  <si>
+    <t>4th</t>
+  </si>
+  <si>
+    <t>2nd Sprint - weeks 4-6</t>
+  </si>
+  <si>
+    <t>3rd Sprint - weeks 7-9</t>
+  </si>
+  <si>
+    <t>4th Sprint - weeks 10-12</t>
+  </si>
+  <si>
+    <t>Integration with Zube.io</t>
+  </si>
+  <si>
+    <t>UML diagram creation</t>
+  </si>
+  <si>
+    <t>Introduction of sprint boards</t>
+  </si>
+  <si>
+    <t>Preparation of first 10 raports</t>
+  </si>
+  <si>
+    <t>2 days</t>
+  </si>
+  <si>
+    <t>1 week</t>
+  </si>
+  <si>
+    <t>Introduction of TDD</t>
+  </si>
+  <si>
+    <t>Unit tests</t>
+  </si>
+  <si>
+    <t>3 weeks</t>
+  </si>
+  <si>
+    <t>Integrating tests with Travis</t>
+  </si>
+  <si>
+    <t>Preparation of remaining 15 raports</t>
+  </si>
+  <si>
+    <t>Bug reporting system</t>
+  </si>
+  <si>
+    <t>Deployment working</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -116,8 +177,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -136,13 +200,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D13" totalsRowShown="0">
-  <autoFilter ref="A1:D13"/>
-  <tableColumns count="4">
-    <tableColumn id="1" name="Problem"/>
-    <tableColumn id="2" name="ID"/>
-    <tableColumn id="3" name="Estimation (Time for task)"/>
-    <tableColumn id="4" name="Priority"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:E41" totalsRowShown="0">
+  <autoFilter ref="A1:E41" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Problem"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="ID"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Estimation (Time for task)"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Priority"/>
+    <tableColumn id="5" xr3:uid="{EBBBAB75-AE14-40A7-B86D-B24AA32CA849}" name="Sprint"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -410,21 +475,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="34" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
     <col min="3" max="3" width="25.85546875" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" customWidth="1"/>
+    <col min="7" max="7" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -437,8 +504,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -451,8 +521,14 @@
       <c r="D2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -460,13 +536,19 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -474,13 +556,19 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -488,77 +576,254 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D5">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D6">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
       <c r="D7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
       <c r="D8">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D9">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="E9" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16">
+        <v>13</v>
+      </c>
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18">
+        <v>15</v>
+      </c>
+      <c r="C18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18">
+        <v>4</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19">
+        <v>16</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21">
         <v>17</v>
       </c>
-      <c r="B10">
-        <v>9</v>
-      </c>
-      <c r="C10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10">
-        <v>8</v>
+      <c r="C21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22">
+        <v>19</v>
+      </c>
+      <c r="C22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>